<commit_message>
Started statistics per country
</commit_message>
<xml_diff>
--- a/country_codes.xlsx
+++ b/country_codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wwwgi\Documents\Coding stuff\esc_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B3A96D-9150-42E8-B9F9-EECBCAE2250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B69CA9-DD7F-4A13-B62B-11D944FAEFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{C9FC3F0C-62CC-4996-9526-23727E73FFFD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C9FC3F0C-62CC-4996-9526-23727E73FFFD}"/>
   </bookViews>
   <sheets>
     <sheet name="all_codes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="137">
   <si>
     <t>Netherlands</t>
   </si>
@@ -431,6 +431,12 @@
   </si>
   <si>
     <t>Amami se vuoi</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
@@ -785,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D2F3D0-9FBC-41C6-8FFD-E9C45BAA6ED4}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,367 +809,427 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="1" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G14" s="1" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1179,7 +1245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E43ED3C-1E05-4934-A23D-2BAA723898D3}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>